<commit_message>
Reorgs, devices designations, and stock part selection
git-svn-id: svn+ssh://bbfs-01.calit2.net/grw/Gordon/svn/trunk/Gadgets/Libraries/Parts@21550 2cf53259-273a-af40-bda6-69d31023b8ec
</commit_message>
<xml_diff>
--- a/Digikey/Buttons-Switches.xlsx
+++ b/Digikey/Buttons-Switches.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephen Deiss\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25317"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27960" windowHeight="10260"/>
+    <workbookView xWindow="-20" yWindow="1780" windowWidth="28880" windowHeight="13000"/>
   </bookViews>
   <sheets>
-    <sheet name="SMD-PB" sheetId="1" r:id="rId1"/>
-    <sheet name="TH-PB" sheetId="2" r:id="rId2"/>
+    <sheet name="Buttons-SMD" sheetId="1" r:id="rId1"/>
+    <sheet name="Buttons-TH" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="165">
   <si>
     <t>Datasheets</t>
   </si>
@@ -479,13 +479,49 @@
   </si>
   <si>
     <t>TE_FSM1LPATR</t>
+  </si>
+  <si>
+    <t>PTS525</t>
+  </si>
+  <si>
+    <t>1.50mm</t>
+  </si>
+  <si>
+    <t>5.25mm x 5.25mm</t>
+  </si>
+  <si>
+    <t>CKN9104CT-NDP</t>
+  </si>
+  <si>
+    <t>TS525SM15SMTR2</t>
+  </si>
+  <si>
+    <t>LFS C&amp;K Components</t>
+  </si>
+  <si>
+    <t>http://media.digikey.com/pdf/Data%20Sheets/C&amp;K/PTS525_Series_RevJul_2012.pdf</t>
+  </si>
+  <si>
+    <t>http://media.digikey.com/photos/CK%20Comp%20Photos/PTS525SM10SMTR_sml.jpg</t>
+  </si>
+  <si>
+    <t>TH-VERTICAL</t>
+  </si>
+  <si>
+    <t>SMD-VERTICAL</t>
+  </si>
+  <si>
+    <t>SMD-RIGHT-ANGLE2</t>
+  </si>
+  <si>
+    <t>SMD-RIGHT-ANGLE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -624,6 +660,21 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -926,7 +977,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -970,15 +1021,58 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="85">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1007,6 +1101,48 @@
     <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
@@ -1079,7 +1215,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1114,7 +1250,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1291,7 +1427,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1299,27 +1435,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF10"/>
+  <dimension ref="A1:AF9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="Z6" sqref="Z6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="3" width="16.5703125" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" customWidth="1"/>
-    <col min="6" max="6" width="17.140625" customWidth="1"/>
-    <col min="12" max="12" width="15.28515625" customWidth="1"/>
-    <col min="13" max="13" width="16.42578125" customWidth="1"/>
-    <col min="16" max="16" width="16.140625" customWidth="1"/>
-    <col min="22" max="22" width="16.85546875" customWidth="1"/>
-    <col min="27" max="27" width="14.28515625" customWidth="1"/>
-    <col min="31" max="31" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16.5" customWidth="1"/>
+    <col min="4" max="4" width="20.5" customWidth="1"/>
+    <col min="5" max="5" width="19.5" customWidth="1"/>
+    <col min="6" max="6" width="39.83203125" customWidth="1"/>
+    <col min="12" max="12" width="15.33203125" customWidth="1"/>
+    <col min="13" max="13" width="16.5" customWidth="1"/>
+    <col min="16" max="16" width="16.1640625" customWidth="1"/>
+    <col min="22" max="22" width="16.83203125" customWidth="1"/>
+    <col min="27" max="27" width="14.33203125" customWidth="1"/>
+    <col min="31" max="31" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1417,7 +1553,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32">
       <c r="A2" s="1" t="s">
         <v>28</v>
       </c>
@@ -1502,11 +1638,17 @@
       <c r="AB2" t="s">
         <v>43</v>
       </c>
+      <c r="AC2" t="s">
+        <v>93</v>
+      </c>
       <c r="AE2" s="2" t="s">
         <v>149</v>
       </c>
+      <c r="AF2" t="s">
+        <v>162</v>
+      </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -1591,11 +1733,17 @@
       <c r="AB3" t="s">
         <v>43</v>
       </c>
+      <c r="AC3" t="s">
+        <v>93</v>
+      </c>
       <c r="AE3" t="s">
         <v>149</v>
       </c>
+      <c r="AF3" t="s">
+        <v>162</v>
+      </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -1680,11 +1828,17 @@
       <c r="AB4" t="s">
         <v>43</v>
       </c>
+      <c r="AC4" t="s">
+        <v>93</v>
+      </c>
       <c r="AE4" t="s">
         <v>149</v>
       </c>
+      <c r="AF4" t="s">
+        <v>162</v>
+      </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -1769,11 +1923,17 @@
       <c r="AB5" t="s">
         <v>43</v>
       </c>
+      <c r="AC5" t="s">
+        <v>93</v>
+      </c>
       <c r="AE5" t="s">
         <v>149</v>
       </c>
+      <c r="AF5" t="s">
+        <v>162</v>
+      </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32">
       <c r="A6" t="s">
         <v>117</v>
       </c>
@@ -1862,33 +2022,217 @@
         <v>152</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32">
+      <c r="A7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D7" t="s">
+        <v>100</v>
+      </c>
+      <c r="E7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" t="s">
+        <v>101</v>
+      </c>
+      <c r="G7">
+        <v>10626</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>2.69</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7" t="s">
+        <v>102</v>
+      </c>
+      <c r="M7" t="s">
+        <v>43</v>
+      </c>
+      <c r="N7" t="s">
+        <v>33</v>
+      </c>
+      <c r="O7" t="s">
+        <v>34</v>
+      </c>
+      <c r="P7" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>104</v>
+      </c>
+      <c r="R7" t="s">
+        <v>105</v>
+      </c>
+      <c r="S7" t="s">
+        <v>43</v>
+      </c>
+      <c r="T7" t="s">
+        <v>106</v>
+      </c>
+      <c r="U7" t="s">
+        <v>40</v>
+      </c>
+      <c r="V7" t="s">
+        <v>107</v>
+      </c>
+      <c r="W7" t="s">
+        <v>42</v>
+      </c>
+      <c r="X7" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>108</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>150</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32">
+      <c r="A8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B8" t="s">
+        <v>110</v>
+      </c>
+      <c r="C8" t="s">
+        <v>111</v>
+      </c>
+      <c r="D8" t="s">
+        <v>112</v>
+      </c>
+      <c r="E8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>1.02</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8" t="s">
+        <v>102</v>
+      </c>
+      <c r="M8" t="s">
+        <v>43</v>
+      </c>
+      <c r="N8" t="s">
+        <v>33</v>
+      </c>
+      <c r="O8" t="s">
+        <v>34</v>
+      </c>
+      <c r="P8" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>36</v>
+      </c>
+      <c r="R8" t="s">
+        <v>105</v>
+      </c>
+      <c r="S8" t="s">
+        <v>43</v>
+      </c>
+      <c r="T8" t="s">
+        <v>106</v>
+      </c>
+      <c r="U8" t="s">
+        <v>113</v>
+      </c>
+      <c r="V8" t="s">
+        <v>114</v>
+      </c>
+      <c r="W8" t="s">
+        <v>42</v>
+      </c>
+      <c r="X8" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>115</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>116</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>151</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32">
       <c r="A9" t="s">
-        <v>97</v>
+        <v>159</v>
       </c>
       <c r="B9" t="s">
-        <v>98</v>
+        <v>160</v>
       </c>
       <c r="C9" t="s">
-        <v>99</v>
+        <v>156</v>
       </c>
       <c r="D9" t="s">
-        <v>100</v>
+        <v>157</v>
       </c>
       <c r="E9" t="s">
-        <v>30</v>
+        <v>158</v>
       </c>
       <c r="F9" t="s">
         <v>101</v>
       </c>
       <c r="G9">
-        <v>10626</v>
+        <v>2726</v>
       </c>
       <c r="H9">
         <v>0</v>
       </c>
       <c r="I9">
-        <v>2.69</v>
+        <v>0.65</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -1900,7 +2244,7 @@
         <v>102</v>
       </c>
       <c r="M9" t="s">
-        <v>43</v>
+        <v>153</v>
       </c>
       <c r="N9" t="s">
         <v>33</v>
@@ -1912,22 +2256,22 @@
         <v>103</v>
       </c>
       <c r="Q9" t="s">
-        <v>104</v>
+        <v>36</v>
       </c>
       <c r="R9" t="s">
-        <v>105</v>
+        <v>37</v>
       </c>
       <c r="S9" t="s">
-        <v>43</v>
+        <v>154</v>
       </c>
       <c r="T9" t="s">
-        <v>106</v>
+        <v>39</v>
       </c>
       <c r="U9" t="s">
         <v>40</v>
       </c>
       <c r="V9" t="s">
-        <v>107</v>
+        <v>155</v>
       </c>
       <c r="W9" t="s">
         <v>42</v>
@@ -1939,105 +2283,13 @@
         <v>43</v>
       </c>
       <c r="Z9" t="s">
-        <v>108</v>
+        <v>44</v>
       </c>
       <c r="AA9" t="s">
         <v>43</v>
       </c>
       <c r="AB9" t="s">
         <v>43</v>
-      </c>
-      <c r="AE9" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>109</v>
-      </c>
-      <c r="B10" t="s">
-        <v>110</v>
-      </c>
-      <c r="C10" t="s">
-        <v>111</v>
-      </c>
-      <c r="D10" t="s">
-        <v>112</v>
-      </c>
-      <c r="E10" t="s">
-        <v>30</v>
-      </c>
-      <c r="F10" t="s">
-        <v>31</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>1.02</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10">
-        <v>1</v>
-      </c>
-      <c r="L10" t="s">
-        <v>102</v>
-      </c>
-      <c r="M10" t="s">
-        <v>43</v>
-      </c>
-      <c r="N10" t="s">
-        <v>33</v>
-      </c>
-      <c r="O10" t="s">
-        <v>34</v>
-      </c>
-      <c r="P10" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>36</v>
-      </c>
-      <c r="R10" t="s">
-        <v>105</v>
-      </c>
-      <c r="S10" t="s">
-        <v>43</v>
-      </c>
-      <c r="T10" t="s">
-        <v>106</v>
-      </c>
-      <c r="U10" t="s">
-        <v>113</v>
-      </c>
-      <c r="V10" t="s">
-        <v>114</v>
-      </c>
-      <c r="W10" t="s">
-        <v>42</v>
-      </c>
-      <c r="X10" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y10" t="s">
-        <v>43</v>
-      </c>
-      <c r="Z10" t="s">
-        <v>46</v>
-      </c>
-      <c r="AA10" t="s">
-        <v>115</v>
-      </c>
-      <c r="AB10" t="s">
-        <v>116</v>
-      </c>
-      <c r="AE10" t="s">
-        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -2045,26 +2297,31 @@
     <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF16"/>
+  <dimension ref="A1:AF14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="AF5" sqref="AF5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="3" width="18.28515625" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" customWidth="1"/>
-    <col min="22" max="22" width="20.5703125" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" customWidth="1"/>
+    <col min="22" max="22" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2162,7 +2419,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32">
       <c r="A2" t="s">
         <v>61</v>
       </c>
@@ -2247,11 +2504,17 @@
       <c r="AB2" t="s">
         <v>43</v>
       </c>
+      <c r="AC2" t="s">
+        <v>93</v>
+      </c>
       <c r="AE2" t="s">
         <v>147</v>
       </c>
+      <c r="AF2" t="s">
+        <v>161</v>
+      </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32">
       <c r="A3" t="s">
         <v>61</v>
       </c>
@@ -2336,11 +2599,17 @@
       <c r="AB3" t="s">
         <v>43</v>
       </c>
+      <c r="AC3" t="s">
+        <v>93</v>
+      </c>
       <c r="AE3" t="s">
         <v>147</v>
       </c>
+      <c r="AF3" t="s">
+        <v>161</v>
+      </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32">
       <c r="A4" t="s">
         <v>61</v>
       </c>
@@ -2425,11 +2694,17 @@
       <c r="AB4" t="s">
         <v>43</v>
       </c>
+      <c r="AC4" t="s">
+        <v>93</v>
+      </c>
       <c r="AE4" t="s">
         <v>147</v>
       </c>
+      <c r="AF4" t="s">
+        <v>161</v>
+      </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32">
       <c r="A5" t="s">
         <v>61</v>
       </c>
@@ -2514,11 +2789,17 @@
       <c r="AB5" t="s">
         <v>43</v>
       </c>
+      <c r="AC5" t="s">
+        <v>93</v>
+      </c>
       <c r="AE5" t="s">
         <v>147</v>
       </c>
+      <c r="AF5" t="s">
+        <v>161</v>
+      </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32">
       <c r="A6" t="s">
         <v>61</v>
       </c>
@@ -2603,11 +2884,17 @@
       <c r="AB6" t="s">
         <v>43</v>
       </c>
+      <c r="AC6" t="s">
+        <v>93</v>
+      </c>
       <c r="AE6" t="s">
         <v>147</v>
       </c>
+      <c r="AF6" t="s">
+        <v>161</v>
+      </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32">
       <c r="A7" t="s">
         <v>61</v>
       </c>
@@ -2692,11 +2979,17 @@
       <c r="AB7" t="s">
         <v>43</v>
       </c>
+      <c r="AC7" t="s">
+        <v>93</v>
+      </c>
       <c r="AE7" t="s">
         <v>147</v>
       </c>
+      <c r="AF7" t="s">
+        <v>161</v>
+      </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32">
       <c r="A8" t="s">
         <v>61</v>
       </c>
@@ -2784,8 +3077,11 @@
       <c r="AE8" t="s">
         <v>147</v>
       </c>
+      <c r="AF8" t="s">
+        <v>161</v>
+      </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32">
       <c r="A9" t="s">
         <v>61</v>
       </c>
@@ -2870,20 +3166,215 @@
       <c r="AB9" t="s">
         <v>43</v>
       </c>
-      <c r="AE9" s="2"/>
+      <c r="AE9" t="s">
+        <v>147</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>161</v>
+      </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32">
+      <c r="A10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B10" t="s">
+        <v>124</v>
+      </c>
+      <c r="C10" t="s">
+        <v>125</v>
+      </c>
+      <c r="D10" t="s">
+        <v>126</v>
+      </c>
+      <c r="E10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10">
+        <v>55245</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0.16</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10" t="s">
+        <v>51</v>
+      </c>
+      <c r="M10" t="s">
+        <v>127</v>
+      </c>
+      <c r="N10" t="s">
+        <v>33</v>
+      </c>
+      <c r="O10" t="s">
+        <v>34</v>
+      </c>
+      <c r="P10" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>36</v>
+      </c>
+      <c r="R10" t="s">
+        <v>128</v>
+      </c>
+      <c r="S10" t="s">
+        <v>129</v>
+      </c>
+      <c r="T10" t="s">
+        <v>106</v>
+      </c>
+      <c r="U10" t="s">
+        <v>67</v>
+      </c>
+      <c r="V10" t="s">
+        <v>130</v>
+      </c>
+      <c r="W10" t="s">
+        <v>42</v>
+      </c>
+      <c r="X10" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>93</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>148</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32">
+      <c r="A11" t="s">
+        <v>123</v>
+      </c>
+      <c r="B11" t="s">
+        <v>131</v>
+      </c>
+      <c r="C11" t="s">
+        <v>132</v>
+      </c>
+      <c r="D11" t="s">
+        <v>133</v>
+      </c>
+      <c r="E11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11">
+        <v>23047</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11" t="s">
+        <v>51</v>
+      </c>
+      <c r="M11" t="s">
+        <v>127</v>
+      </c>
+      <c r="N11" t="s">
+        <v>33</v>
+      </c>
+      <c r="O11" t="s">
+        <v>34</v>
+      </c>
+      <c r="P11" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>36</v>
+      </c>
+      <c r="R11" t="s">
+        <v>128</v>
+      </c>
+      <c r="S11" t="s">
+        <v>134</v>
+      </c>
+      <c r="T11" t="s">
+        <v>106</v>
+      </c>
+      <c r="U11" t="s">
+        <v>67</v>
+      </c>
+      <c r="V11" t="s">
+        <v>130</v>
+      </c>
+      <c r="W11" t="s">
+        <v>42</v>
+      </c>
+      <c r="X11" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>93</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>148</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32">
       <c r="A12" t="s">
         <v>123</v>
       </c>
       <c r="B12" t="s">
-        <v>124</v>
-      </c>
-      <c r="C12" t="s">
-        <v>125</v>
+        <v>135</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>136</v>
       </c>
       <c r="D12" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="E12" t="s">
         <v>30</v>
@@ -2892,13 +3383,13 @@
         <v>31</v>
       </c>
       <c r="G12">
-        <v>55245</v>
+        <v>16488</v>
       </c>
       <c r="H12">
         <v>0</v>
       </c>
       <c r="I12">
-        <v>0.16</v>
+        <v>0.18</v>
       </c>
       <c r="J12">
         <v>0</v>
@@ -2928,7 +3419,7 @@
         <v>128</v>
       </c>
       <c r="S12" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="T12" t="s">
         <v>106</v>
@@ -2957,22 +3448,28 @@
       <c r="AB12" t="s">
         <v>43</v>
       </c>
+      <c r="AC12" t="s">
+        <v>93</v>
+      </c>
       <c r="AE12" t="s">
         <v>148</v>
       </c>
+      <c r="AF12" t="s">
+        <v>161</v>
+      </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:32">
       <c r="A13" t="s">
         <v>123</v>
       </c>
       <c r="B13" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="C13" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="D13" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="E13" t="s">
         <v>30</v>
@@ -2981,13 +3478,13 @@
         <v>31</v>
       </c>
       <c r="G13">
-        <v>23047</v>
+        <v>38978</v>
       </c>
       <c r="H13">
         <v>0</v>
       </c>
       <c r="I13">
-        <v>0.14000000000000001</v>
+        <v>0.23</v>
       </c>
       <c r="J13">
         <v>0</v>
@@ -3017,7 +3514,7 @@
         <v>128</v>
       </c>
       <c r="S13" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="T13" t="s">
         <v>106</v>
@@ -3046,37 +3543,43 @@
       <c r="AB13" t="s">
         <v>43</v>
       </c>
+      <c r="AC13" t="s">
+        <v>93</v>
+      </c>
       <c r="AE13" t="s">
         <v>148</v>
       </c>
+      <c r="AF13" t="s">
+        <v>161</v>
+      </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:32">
       <c r="A14" t="s">
         <v>123</v>
       </c>
       <c r="B14" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="C14" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="D14" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="E14" t="s">
-        <v>30</v>
+        <v>146</v>
       </c>
       <c r="F14" t="s">
         <v>31</v>
       </c>
       <c r="G14">
-        <v>16488</v>
+        <v>3379</v>
       </c>
       <c r="H14">
         <v>0</v>
       </c>
       <c r="I14">
-        <v>0.18</v>
+        <v>0.33</v>
       </c>
       <c r="J14">
         <v>0</v>
@@ -3106,7 +3609,7 @@
         <v>128</v>
       </c>
       <c r="S14" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="T14" t="s">
         <v>106</v>
@@ -3127,7 +3630,7 @@
         <v>43</v>
       </c>
       <c r="Z14" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="AA14" t="s">
         <v>43</v>
@@ -3138,187 +3641,17 @@
       <c r="AE14" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>123</v>
-      </c>
-      <c r="B15" t="s">
-        <v>139</v>
-      </c>
-      <c r="C15" t="s">
-        <v>140</v>
-      </c>
-      <c r="D15" t="s">
-        <v>141</v>
-      </c>
-      <c r="E15" t="s">
-        <v>30</v>
-      </c>
-      <c r="F15" t="s">
-        <v>31</v>
-      </c>
-      <c r="G15">
-        <v>38978</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <v>0.23</v>
-      </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
-      <c r="K15">
-        <v>1</v>
-      </c>
-      <c r="L15" t="s">
-        <v>51</v>
-      </c>
-      <c r="M15" t="s">
-        <v>127</v>
-      </c>
-      <c r="N15" t="s">
-        <v>33</v>
-      </c>
-      <c r="O15" t="s">
-        <v>34</v>
-      </c>
-      <c r="P15" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>36</v>
-      </c>
-      <c r="R15" t="s">
-        <v>128</v>
-      </c>
-      <c r="S15" t="s">
-        <v>142</v>
-      </c>
-      <c r="T15" t="s">
-        <v>106</v>
-      </c>
-      <c r="U15" t="s">
-        <v>67</v>
-      </c>
-      <c r="V15" t="s">
-        <v>130</v>
-      </c>
-      <c r="W15" t="s">
-        <v>42</v>
-      </c>
-      <c r="X15" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y15" t="s">
-        <v>43</v>
-      </c>
-      <c r="Z15" t="s">
-        <v>44</v>
-      </c>
-      <c r="AA15" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB15" t="s">
-        <v>43</v>
-      </c>
-      <c r="AE15" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>123</v>
-      </c>
-      <c r="B16" t="s">
-        <v>143</v>
-      </c>
-      <c r="C16" t="s">
-        <v>144</v>
-      </c>
-      <c r="D16" t="s">
-        <v>145</v>
-      </c>
-      <c r="E16" t="s">
-        <v>146</v>
-      </c>
-      <c r="F16" t="s">
-        <v>31</v>
-      </c>
-      <c r="G16">
-        <v>3379</v>
-      </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-      <c r="I16">
-        <v>0.33</v>
-      </c>
-      <c r="J16">
-        <v>0</v>
-      </c>
-      <c r="K16">
-        <v>1</v>
-      </c>
-      <c r="L16" t="s">
-        <v>51</v>
-      </c>
-      <c r="M16" t="s">
-        <v>127</v>
-      </c>
-      <c r="N16" t="s">
-        <v>33</v>
-      </c>
-      <c r="O16" t="s">
-        <v>34</v>
-      </c>
-      <c r="P16" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>36</v>
-      </c>
-      <c r="R16" t="s">
-        <v>128</v>
-      </c>
-      <c r="S16" t="s">
-        <v>129</v>
-      </c>
-      <c r="T16" t="s">
-        <v>106</v>
-      </c>
-      <c r="U16" t="s">
-        <v>67</v>
-      </c>
-      <c r="V16" t="s">
-        <v>130</v>
-      </c>
-      <c r="W16" t="s">
-        <v>42</v>
-      </c>
-      <c r="X16" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y16" t="s">
-        <v>43</v>
-      </c>
-      <c r="Z16" t="s">
-        <v>46</v>
-      </c>
-      <c r="AA16" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB16" t="s">
-        <v>43</v>
-      </c>
-      <c r="AE16" t="s">
-        <v>148</v>
+      <c r="AF14" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added pushbutton requested long ago
git-svn-id: svn+ssh://bbfs-01.calit2.net/grw/Gordon/svn/trunk/Gadgets/Libraries/Parts@22257 2cf53259-273a-af40-bda6-69d31023b8ec
</commit_message>
<xml_diff>
--- a/Digikey/Buttons-Switches.xlsx
+++ b/Digikey/Buttons-Switches.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25317"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\PCB Libraries\Library Expert 2015\Libraries\NVSL-Footprint-Library\Eagle\DigiKey\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="1780" windowWidth="28880" windowHeight="13000"/>
+    <workbookView xWindow="-15" yWindow="1785" windowWidth="28875" windowHeight="13005"/>
   </bookViews>
   <sheets>
     <sheet name="Buttons-SMD" sheetId="1" r:id="rId1"/>
@@ -20,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="167">
   <si>
     <t>Datasheets</t>
   </si>
@@ -493,9 +498,6 @@
     <t>CKN9104CT-NDP</t>
   </si>
   <si>
-    <t>TS525SM15SMTR2</t>
-  </si>
-  <si>
     <t>LFS C&amp;K Components</t>
   </si>
   <si>
@@ -515,6 +517,15 @@
   </si>
   <si>
     <t>SMD-RIGHT-ANGLE</t>
+  </si>
+  <si>
+    <t>PTS525SM15SMTR2</t>
+  </si>
+  <si>
+    <t>CK_PTS525SM10SMTRLFS_HS</t>
+  </si>
+  <si>
+    <t>SMD-VERTICAL2</t>
   </si>
 </sst>
 </file>
@@ -1427,7 +1438,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1437,25 +1448,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="Z6" sqref="Z6"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="AE18" sqref="AE18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="16.5" customWidth="1"/>
-    <col min="4" max="4" width="20.5" customWidth="1"/>
-    <col min="5" max="5" width="19.5" customWidth="1"/>
-    <col min="6" max="6" width="39.83203125" customWidth="1"/>
-    <col min="12" max="12" width="15.33203125" customWidth="1"/>
-    <col min="13" max="13" width="16.5" customWidth="1"/>
-    <col min="16" max="16" width="16.1640625" customWidth="1"/>
-    <col min="22" max="22" width="16.83203125" customWidth="1"/>
-    <col min="27" max="27" width="14.33203125" customWidth="1"/>
-    <col min="31" max="31" width="13.83203125" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" customWidth="1"/>
+    <col min="6" max="6" width="39.85546875" customWidth="1"/>
+    <col min="12" max="12" width="15.28515625" customWidth="1"/>
+    <col min="13" max="13" width="16.42578125" customWidth="1"/>
+    <col min="16" max="16" width="16.140625" customWidth="1"/>
+    <col min="22" max="22" width="16.85546875" customWidth="1"/>
+    <col min="27" max="27" width="14.28515625" customWidth="1"/>
+    <col min="31" max="31" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1553,7 +1564,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:32">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>28</v>
       </c>
@@ -1645,10 +1656,10 @@
         <v>149</v>
       </c>
       <c r="AF2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
-    <row r="3" spans="1:32">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -1740,10 +1751,10 @@
         <v>149</v>
       </c>
       <c r="AF3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
-    <row r="4" spans="1:32">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -1835,10 +1846,10 @@
         <v>149</v>
       </c>
       <c r="AF4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
-    <row r="5" spans="1:32">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -1930,10 +1941,10 @@
         <v>149</v>
       </c>
       <c r="AF5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
-    <row r="6" spans="1:32">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>117</v>
       </c>
@@ -2022,7 +2033,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="7" spans="1:32">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>97</v>
       </c>
@@ -2111,10 +2122,10 @@
         <v>150</v>
       </c>
       <c r="AF7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
-    <row r="8" spans="1:32">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>109</v>
       </c>
@@ -2203,24 +2214,24 @@
         <v>151</v>
       </c>
       <c r="AF8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
-    <row r="9" spans="1:32">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>158</v>
+      </c>
+      <c r="B9" t="s">
         <v>159</v>
-      </c>
-      <c r="B9" t="s">
-        <v>160</v>
       </c>
       <c r="C9" t="s">
         <v>156</v>
       </c>
       <c r="D9" t="s">
+        <v>164</v>
+      </c>
+      <c r="E9" t="s">
         <v>157</v>
-      </c>
-      <c r="E9" t="s">
-        <v>158</v>
       </c>
       <c r="F9" t="s">
         <v>101</v>
@@ -2290,6 +2301,12 @@
       </c>
       <c r="AB9" t="s">
         <v>43</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>165</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -2297,7 +2314,7 @@
     <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2314,14 +2331,14 @@
       <selection activeCell="AF5" sqref="AF5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="18.33203125" customWidth="1"/>
-    <col min="4" max="4" width="15.1640625" customWidth="1"/>
-    <col min="22" max="22" width="20.5" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" customWidth="1"/>
+    <col min="22" max="22" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2419,7 +2436,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:32">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>61</v>
       </c>
@@ -2511,10 +2528,10 @@
         <v>147</v>
       </c>
       <c r="AF2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:32">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>61</v>
       </c>
@@ -2606,10 +2623,10 @@
         <v>147</v>
       </c>
       <c r="AF3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
-    <row r="4" spans="1:32">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>61</v>
       </c>
@@ -2701,10 +2718,10 @@
         <v>147</v>
       </c>
       <c r="AF4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
-    <row r="5" spans="1:32">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>61</v>
       </c>
@@ -2796,10 +2813,10 @@
         <v>147</v>
       </c>
       <c r="AF5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
-    <row r="6" spans="1:32">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>61</v>
       </c>
@@ -2891,10 +2908,10 @@
         <v>147</v>
       </c>
       <c r="AF6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
-    <row r="7" spans="1:32">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>61</v>
       </c>
@@ -2986,10 +3003,10 @@
         <v>147</v>
       </c>
       <c r="AF7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
-    <row r="8" spans="1:32">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>61</v>
       </c>
@@ -3078,10 +3095,10 @@
         <v>147</v>
       </c>
       <c r="AF8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
-    <row r="9" spans="1:32">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>61</v>
       </c>
@@ -3170,10 +3187,10 @@
         <v>147</v>
       </c>
       <c r="AF9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
-    <row r="10" spans="1:32">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>123</v>
       </c>
@@ -3265,10 +3282,10 @@
         <v>148</v>
       </c>
       <c r="AF10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
-    <row r="11" spans="1:32">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>123</v>
       </c>
@@ -3360,10 +3377,10 @@
         <v>148</v>
       </c>
       <c r="AF11" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
-    <row r="12" spans="1:32">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>123</v>
       </c>
@@ -3455,10 +3472,10 @@
         <v>148</v>
       </c>
       <c r="AF12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
-    <row r="13" spans="1:32">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>123</v>
       </c>
@@ -3550,10 +3567,10 @@
         <v>148</v>
       </c>
       <c r="AF13" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
-    <row r="14" spans="1:32">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>123</v>
       </c>
@@ -3642,7 +3659,7 @@
         <v>148</v>
       </c>
       <c r="AF14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>